<commit_message>
Updated the graphic labels and excel doc.
</commit_message>
<xml_diff>
--- a/results/results_analysis.xlsx
+++ b/results/results_analysis.xlsx
@@ -348,7 +348,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Fairness of Matchings</a:t>
+              <a:t>Average Fairness within</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> a </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Matching</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -673,11 +681,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="448017744"/>
-        <c:axId val="442188456"/>
+        <c:axId val="218572240"/>
+        <c:axId val="218572632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="448017744"/>
+        <c:axId val="218572240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -720,7 +728,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442188456"/>
+        <c:crossAx val="218572632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -728,7 +736,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="442188456"/>
+        <c:axId val="218572632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -774,7 +782,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of Total Cost</a:t>
+                  <a:t> of Total Matching Score</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -840,7 +848,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448017744"/>
+        <c:crossAx val="218572240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1286,11 +1294,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="448988360"/>
-        <c:axId val="448988752"/>
+        <c:axId val="218573416"/>
+        <c:axId val="218573808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="448988360"/>
+        <c:axId val="218573416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1333,7 +1341,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448988752"/>
+        <c:crossAx val="218573808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1341,7 +1349,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448988752"/>
+        <c:axId val="218573808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1383,7 +1391,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Percent of Pessimal Cost</a:t>
+                  <a:t>Percent of Pessimal Group Score</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1449,7 +1457,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448988360"/>
+        <c:crossAx val="218573416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8981,7 +8989,7 @@
         <v>176091</v>
       </c>
       <c r="O70">
-        <f t="shared" ref="O70:P72" si="3">(K70-C70)/(G70-C70)</f>
+        <f t="shared" ref="O70:O72" si="3">(K70-C70)/(G70-C70)</f>
         <v>0.12119438338771554</v>
       </c>
       <c r="P70">
@@ -9176,8 +9184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G4:W19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AA19" sqref="AA19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>